<commit_message>
Made changes in the document, added comment for Facebook SDK missing.
</commit_message>
<xml_diff>
--- a/FacebookCompleteAPI/Documents/FaceBookComponent.xlsx
+++ b/FacebookCompleteAPI/Documents/FaceBookComponent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -277,9 +277,6 @@
     <t>Like Post' method will like any post/feed. Post Id is passed an an parameter.</t>
   </si>
   <si>
-    <t>Facebook SDK 3.1</t>
-  </si>
-  <si>
     <t>This components works for both iOS 5 and iOS 6.</t>
   </si>
   <si>
@@ -289,16 +286,7 @@
     <t>Using facebook SDK 3.1 (latest sdk) for communicating with facebook API</t>
   </si>
   <si>
-    <t>AdSupport.framework (marked as optional)</t>
-  </si>
-  <si>
-    <t>Social.framework (marked as optional)</t>
-  </si>
-  <si>
     <t>libsqlite3.0.dylib</t>
-  </si>
-  <si>
-    <t>Accounts.framework (marked as optional)</t>
   </si>
   <si>
     <t>Client Application</t>
@@ -389,6 +377,94 @@
     <t>Create a facebook app id and enter that app id in 'project-name'-info.plist file.
 Add a URLTypes to the same 'project-name'-info.plist file by attaching fb keyword to the app id.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Facebook SDK 3.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(if u r cloning a fresh code copy from git hub, then in case please install facebook SDK frm developer.facebook.com and add facebook.framework in your code)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Accounts.framework</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (marked as optional)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">AdSupport.framework </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(marked as optional)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Social.framework</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (marked as optional)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -401,7 +477,7 @@
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +618,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -625,7 +708,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="40">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -700,6 +783,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -715,7 +802,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,6 +940,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -860,54 +960,44 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="40">
+  <cellStyles count="44">
     <cellStyle name="Comma 2" xfId="5"/>
     <cellStyle name="Comma[0]" xfId="6"/>
     <cellStyle name="Currency 2" xfId="3"/>
@@ -928,6 +1018,8 @@
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
@@ -944,6 +1036,8 @@
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -1253,37 +1347,37 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="4" spans="1:7">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1416,7 +1510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1686,7 +1780,7 @@
       <c r="A7" s="32">
         <v>7</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="49" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="16"/>
@@ -1695,7 +1789,7 @@
       <c r="A8" s="32">
         <v>8</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="50" t="s">
         <v>70</v>
       </c>
       <c r="C8" s="36"/>
@@ -1704,7 +1798,7 @@
       <c r="A9" s="32">
         <v>9</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="50" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="36"/>
@@ -1713,7 +1807,7 @@
       <c r="A10" s="32">
         <v>10</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="50" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="36"/>
@@ -1722,7 +1816,7 @@
       <c r="A11" s="32">
         <v>11</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="50" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="36"/>
@@ -1740,7 +1834,7 @@
       <c r="A13" s="32">
         <v>13</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="50" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="36"/>
@@ -1749,7 +1843,7 @@
       <c r="A14" s="32">
         <v>14</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="50" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="36"/>
@@ -1758,7 +1852,7 @@
       <c r="A15" s="32">
         <v>15</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="50" t="s">
         <v>77</v>
       </c>
       <c r="C15" s="36"/>
@@ -1767,7 +1861,7 @@
       <c r="A16" s="32">
         <v>16</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="50" t="s">
         <v>78</v>
       </c>
       <c r="C16" s="36"/>
@@ -1833,176 +1927,202 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:J28"/>
+  <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="6" spans="3:10">
-      <c r="C6" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-    </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-    </row>
-    <row r="9" spans="3:10">
-      <c r="H9" s="67" t="s">
+    <row r="2" spans="2:10">
+      <c r="C2" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+    </row>
+    <row r="6" spans="2:10" ht="14" customHeight="1">
+      <c r="B6" s="51"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="51"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="51"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="51"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="51"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="H9" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="C11" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="C16" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+    </row>
+    <row r="17" spans="3:10">
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+    </row>
+    <row r="18" spans="3:10">
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+    </row>
+    <row r="19" spans="3:10">
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+    </row>
+    <row r="20" spans="3:10">
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+    </row>
+    <row r="21" spans="3:10">
+      <c r="C21" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-    </row>
-    <row r="10" spans="3:10">
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-    </row>
-    <row r="11" spans="3:10">
-      <c r="C11" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-    </row>
-    <row r="12" spans="3:10">
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-    </row>
-    <row r="13" spans="3:10">
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-    </row>
-    <row r="14" spans="3:10">
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-    </row>
-    <row r="15" spans="3:10">
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-    </row>
-    <row r="17" spans="3:10">
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-    </row>
-    <row r="18" spans="3:10">
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-    </row>
-    <row r="19" spans="3:10">
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-    </row>
-    <row r="20" spans="3:10">
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-    </row>
-    <row r="21" spans="3:10">
-      <c r="C21" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
     </row>
     <row r="22" spans="3:10">
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
     </row>
     <row r="23" spans="3:10">
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
     </row>
     <row r="24" spans="3:10">
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
     </row>
     <row r="25" spans="3:10">
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
     </row>
     <row r="26" spans="3:10">
-      <c r="C26" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
+      <c r="C26" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
     </row>
     <row r="27" spans="3:10">
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="28" spans="3:10">
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C26:E28"/>
     <mergeCell ref="H9:J25"/>
-    <mergeCell ref="C6:E8"/>
     <mergeCell ref="C11:E13"/>
     <mergeCell ref="C16:E18"/>
     <mergeCell ref="C21:E23"/>
+    <mergeCell ref="C2:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2025,62 +2145,62 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="3" spans="2:21">
-      <c r="G3" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
+      <c r="G3" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
     </row>
     <row r="4" spans="2:21">
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
     </row>
     <row r="5" spans="2:21">
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="2:21">
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
     </row>
     <row r="7" spans="2:21">
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
     </row>
     <row r="8" spans="2:21">
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
     </row>
     <row r="9" spans="2:21">
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
     </row>
     <row r="10" spans="2:21">
-      <c r="B10" s="64" t="s">
-        <v>87</v>
+      <c r="B10" s="62" t="s">
+        <v>83</v>
       </c>
       <c r="C10" s="63"/>
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="Q10" s="66" t="s">
-        <v>88</v>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="Q10" s="64" t="s">
+        <v>84</v>
       </c>
       <c r="R10" s="65"/>
       <c r="S10" s="65"/>
@@ -2091,90 +2211,90 @@
       <c r="C11" s="63"/>
       <c r="D11" s="63"/>
       <c r="E11" s="63"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="65"/>
       <c r="S11" s="65"/>
       <c r="T11" s="65"/>
-      <c r="U11" s="57"/>
+      <c r="U11" s="51"/>
     </row>
     <row r="12" spans="2:21">
       <c r="B12" s="63"/>
       <c r="C12" s="63"/>
       <c r="D12" s="63"/>
       <c r="E12" s="63"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
       <c r="Q12" s="65"/>
       <c r="R12" s="65"/>
       <c r="S12" s="65"/>
       <c r="T12" s="65"/>
-      <c r="U12" s="57"/>
+      <c r="U12" s="51"/>
     </row>
     <row r="13" spans="2:21">
       <c r="B13" s="63"/>
       <c r="C13" s="63"/>
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
       <c r="Q13" s="65"/>
       <c r="R13" s="65"/>
       <c r="S13" s="65"/>
       <c r="T13" s="65"/>
-      <c r="U13" s="57"/>
+      <c r="U13" s="51"/>
     </row>
     <row r="14" spans="2:21">
       <c r="B14" s="63"/>
       <c r="C14" s="63"/>
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
       <c r="Q14" s="65"/>
       <c r="R14" s="65"/>
       <c r="S14" s="65"/>
       <c r="T14" s="65"/>
-      <c r="U14" s="57"/>
+      <c r="U14" s="51"/>
     </row>
     <row r="15" spans="2:21">
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
       <c r="D15" s="63"/>
       <c r="E15" s="63"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
       <c r="Q15" s="65"/>
       <c r="R15" s="65"/>
       <c r="S15" s="65"/>
       <c r="T15" s="65"/>
-      <c r="U15" s="57"/>
+      <c r="U15" s="51"/>
     </row>
     <row r="16" spans="2:21">
       <c r="B16" s="63"/>
       <c r="C16" s="63"/>
       <c r="D16" s="63"/>
       <c r="E16" s="63"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
       <c r="Q16" s="65"/>
       <c r="R16" s="65"/>
       <c r="S16" s="65"/>
       <c r="T16" s="65"/>
-      <c r="U16" s="57"/>
+      <c r="U16" s="51"/>
     </row>
     <row r="17" spans="2:21">
       <c r="B17" s="63"/>
@@ -2185,7 +2305,7 @@
       <c r="R17" s="65"/>
       <c r="S17" s="65"/>
       <c r="T17" s="65"/>
-      <c r="U17" s="57"/>
+      <c r="U17" s="51"/>
     </row>
     <row r="18" spans="2:21">
       <c r="B18" s="63"/>
@@ -2196,7 +2316,7 @@
       <c r="R18" s="65"/>
       <c r="S18" s="65"/>
       <c r="T18" s="65"/>
-      <c r="U18" s="57"/>
+      <c r="U18" s="51"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="63"/>
@@ -2207,7 +2327,7 @@
       <c r="R19" s="65"/>
       <c r="S19" s="65"/>
       <c r="T19" s="65"/>
-      <c r="U19" s="57"/>
+      <c r="U19" s="51"/>
     </row>
     <row r="20" spans="2:21">
       <c r="B20" s="63"/>
@@ -2218,124 +2338,124 @@
       <c r="R20" s="65"/>
       <c r="S20" s="65"/>
       <c r="T20" s="65"/>
-      <c r="U20" s="57"/>
+      <c r="U20" s="51"/>
     </row>
     <row r="21" spans="2:21">
       <c r="B21" s="63"/>
       <c r="C21" s="63"/>
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
-      <c r="G21" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="58"/>
+      <c r="G21" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="61"/>
+      <c r="N21" s="61"/>
+      <c r="O21" s="61"/>
       <c r="Q21" s="65"/>
       <c r="R21" s="65"/>
       <c r="S21" s="65"/>
       <c r="T21" s="65"/>
-      <c r="U21" s="57"/>
+      <c r="U21" s="51"/>
     </row>
     <row r="22" spans="2:21">
       <c r="B22" s="63"/>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="61"/>
       <c r="Q22" s="65"/>
       <c r="R22" s="65"/>
       <c r="S22" s="65"/>
       <c r="T22" s="65"/>
-      <c r="U22" s="57"/>
+      <c r="U22" s="51"/>
     </row>
     <row r="23" spans="2:21">
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="58"/>
-      <c r="O23" s="58"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
       <c r="Q23" s="65"/>
       <c r="R23" s="65"/>
       <c r="S23" s="65"/>
       <c r="T23" s="65"/>
-      <c r="U23" s="57"/>
+      <c r="U23" s="51"/>
     </row>
     <row r="24" spans="2:21">
       <c r="B24" s="63"/>
       <c r="C24" s="63"/>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="58"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
       <c r="Q24" s="65"/>
       <c r="R24" s="65"/>
       <c r="S24" s="65"/>
       <c r="T24" s="65"/>
-      <c r="U24" s="57"/>
+      <c r="U24" s="51"/>
     </row>
     <row r="25" spans="2:21">
       <c r="B25" s="63"/>
       <c r="C25" s="63"/>
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
       <c r="Q25" s="65"/>
       <c r="R25" s="65"/>
       <c r="S25" s="65"/>
       <c r="T25" s="65"/>
-      <c r="U25" s="57"/>
+      <c r="U25" s="51"/>
     </row>
     <row r="26" spans="2:21">
       <c r="B26" s="63"/>
       <c r="C26" s="63"/>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
       <c r="Q26" s="65"/>
       <c r="R26" s="65"/>
       <c r="S26" s="65"/>
@@ -2346,15 +2466,15 @@
       <c r="C27" s="63"/>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
       <c r="Q27" s="65"/>
       <c r="R27" s="65"/>
       <c r="S27" s="65"/>
@@ -2365,15 +2485,15 @@
       <c r="C28" s="63"/>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="61"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
       <c r="Q28" s="65"/>
       <c r="R28" s="65"/>
       <c r="S28" s="65"/>
@@ -2384,15 +2504,15 @@
       <c r="C29" s="63"/>
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="58"/>
-      <c r="O29" s="58"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="61"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="61"/>
       <c r="Q29" s="65"/>
       <c r="R29" s="65"/>
       <c r="S29" s="65"/>
@@ -2403,15 +2523,15 @@
       <c r="C30" s="63"/>
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="61"/>
+      <c r="M30" s="61"/>
+      <c r="N30" s="61"/>
+      <c r="O30" s="61"/>
       <c r="Q30" s="65"/>
       <c r="R30" s="65"/>
       <c r="S30" s="65"/>
@@ -2422,15 +2542,15 @@
       <c r="C31" s="63"/>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="61"/>
       <c r="Q31" s="65"/>
       <c r="R31" s="65"/>
       <c r="S31" s="65"/>
@@ -2441,15 +2561,15 @@
       <c r="C32" s="63"/>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
       <c r="Q32" s="65"/>
       <c r="R32" s="65"/>
       <c r="S32" s="65"/>
@@ -2460,15 +2580,15 @@
       <c r="C33" s="63"/>
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="61"/>
       <c r="Q33" s="65"/>
       <c r="R33" s="65"/>
       <c r="S33" s="65"/>
@@ -2479,15 +2599,15 @@
       <c r="C34" s="63"/>
       <c r="D34" s="63"/>
       <c r="E34" s="63"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
       <c r="Q34" s="65"/>
       <c r="R34" s="65"/>
       <c r="S34" s="65"/>
@@ -2498,15 +2618,15 @@
       <c r="C35" s="63"/>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="61"/>
       <c r="Q35" s="65"/>
       <c r="R35" s="65"/>
       <c r="S35" s="65"/>
@@ -2517,15 +2637,15 @@
       <c r="C36" s="63"/>
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="58"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="61"/>
+      <c r="L36" s="61"/>
+      <c r="M36" s="61"/>
+      <c r="N36" s="61"/>
+      <c r="O36" s="61"/>
       <c r="Q36" s="65"/>
       <c r="R36" s="65"/>
       <c r="S36" s="65"/>
@@ -2536,15 +2656,15 @@
       <c r="C37" s="63"/>
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="61"/>
       <c r="Q37" s="65"/>
       <c r="R37" s="65"/>
       <c r="S37" s="65"/>
@@ -2555,15 +2675,15 @@
       <c r="C38" s="63"/>
       <c r="D38" s="63"/>
       <c r="E38" s="63"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="58"/>
-      <c r="L38" s="58"/>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58"/>
-      <c r="O38" s="58"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="61"/>
       <c r="Q38" s="65"/>
       <c r="R38" s="65"/>
       <c r="S38" s="65"/>
@@ -2574,15 +2694,15 @@
       <c r="C39" s="63"/>
       <c r="D39" s="63"/>
       <c r="E39" s="63"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="61"/>
+      <c r="O39" s="61"/>
       <c r="Q39" s="65"/>
       <c r="R39" s="65"/>
       <c r="S39" s="65"/>
@@ -2593,15 +2713,15 @@
       <c r="C40" s="63"/>
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="58"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="58"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="61"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="61"/>
+      <c r="O40" s="61"/>
       <c r="Q40" s="65"/>
       <c r="R40" s="65"/>
       <c r="S40" s="65"/>
@@ -2612,1356 +2732,1356 @@
       <c r="C41" s="63"/>
       <c r="D41" s="63"/>
       <c r="E41" s="63"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="58"/>
-      <c r="L41" s="58"/>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+      <c r="L41" s="61"/>
+      <c r="M41" s="61"/>
+      <c r="N41" s="61"/>
+      <c r="O41" s="61"/>
       <c r="Q41" s="65"/>
       <c r="R41" s="65"/>
       <c r="S41" s="65"/>
       <c r="T41" s="65"/>
     </row>
     <row r="42" spans="2:20" ht="14" customHeight="1">
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
-      <c r="O42" s="58"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="61"/>
+      <c r="K42" s="61"/>
+      <c r="L42" s="61"/>
+      <c r="M42" s="61"/>
+      <c r="N42" s="61"/>
+      <c r="O42" s="61"/>
     </row>
     <row r="43" spans="2:20" ht="14" customHeight="1">
-      <c r="C43" s="59"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="61"/>
     </row>
     <row r="44" spans="2:20" ht="14" customHeight="1">
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="58"/>
-      <c r="L44" s="58"/>
-      <c r="M44" s="58"/>
-      <c r="N44" s="58"/>
-      <c r="O44" s="58"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="61"/>
+      <c r="O44" s="61"/>
     </row>
     <row r="45" spans="2:20" ht="14" customHeight="1">
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="61"/>
+      <c r="N45" s="61"/>
+      <c r="O45" s="61"/>
     </row>
     <row r="46" spans="2:20" ht="14" customHeight="1">
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="58"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="61"/>
+      <c r="M46" s="61"/>
+      <c r="N46" s="61"/>
+      <c r="O46" s="61"/>
     </row>
     <row r="47" spans="2:20" ht="14" customHeight="1">
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
+      <c r="M47" s="61"/>
+      <c r="N47" s="61"/>
+      <c r="O47" s="61"/>
     </row>
     <row r="48" spans="2:20" ht="14" customHeight="1">
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="58"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="58"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="61"/>
     </row>
     <row r="49" spans="3:15" ht="14" customHeight="1">
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="58"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="61"/>
+      <c r="L49" s="61"/>
+      <c r="M49" s="61"/>
+      <c r="N49" s="61"/>
+      <c r="O49" s="61"/>
     </row>
     <row r="50" spans="3:15" ht="14" customHeight="1">
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="58"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="61"/>
+      <c r="M50" s="61"/>
+      <c r="N50" s="61"/>
+      <c r="O50" s="61"/>
     </row>
     <row r="51" spans="3:15" ht="14" customHeight="1">
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
-      <c r="L51" s="58"/>
-      <c r="M51" s="58"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="58"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="61"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="61"/>
+      <c r="L51" s="61"/>
+      <c r="M51" s="61"/>
+      <c r="N51" s="61"/>
+      <c r="O51" s="61"/>
     </row>
     <row r="52" spans="3:15" ht="14" customHeight="1">
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="59"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-      <c r="J52" s="58"/>
-      <c r="K52" s="58"/>
-      <c r="L52" s="58"/>
-      <c r="M52" s="58"/>
-      <c r="N52" s="58"/>
-      <c r="O52" s="58"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="G52" s="61"/>
+      <c r="H52" s="61"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="61"/>
+      <c r="K52" s="61"/>
+      <c r="L52" s="61"/>
+      <c r="M52" s="61"/>
+      <c r="N52" s="61"/>
+      <c r="O52" s="61"/>
     </row>
     <row r="53" spans="3:15" ht="14" customHeight="1">
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="58"/>
-      <c r="K53" s="58"/>
-      <c r="L53" s="58"/>
-      <c r="M53" s="58"/>
-      <c r="N53" s="58"/>
-      <c r="O53" s="58"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="G53" s="61"/>
+      <c r="H53" s="61"/>
+      <c r="I53" s="61"/>
+      <c r="J53" s="61"/>
+      <c r="K53" s="61"/>
+      <c r="L53" s="61"/>
+      <c r="M53" s="61"/>
+      <c r="N53" s="61"/>
+      <c r="O53" s="61"/>
     </row>
     <row r="54" spans="3:15" ht="14" customHeight="1">
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="59"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="58"/>
-      <c r="L54" s="58"/>
-      <c r="M54" s="58"/>
-      <c r="N54" s="58"/>
-      <c r="O54" s="58"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="61"/>
+      <c r="I54" s="61"/>
+      <c r="J54" s="61"/>
+      <c r="K54" s="61"/>
+      <c r="L54" s="61"/>
+      <c r="M54" s="61"/>
+      <c r="N54" s="61"/>
+      <c r="O54" s="61"/>
     </row>
     <row r="55" spans="3:15" ht="14" customHeight="1">
-      <c r="C55" s="59"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="58"/>
-      <c r="J55" s="58"/>
-      <c r="K55" s="58"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="58"/>
-      <c r="N55" s="58"/>
-      <c r="O55" s="58"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="61"/>
+      <c r="H55" s="61"/>
+      <c r="I55" s="61"/>
+      <c r="J55" s="61"/>
+      <c r="K55" s="61"/>
+      <c r="L55" s="61"/>
+      <c r="M55" s="61"/>
+      <c r="N55" s="61"/>
+      <c r="O55" s="61"/>
     </row>
     <row r="56" spans="3:15" ht="14" customHeight="1">
-      <c r="C56" s="59"/>
-      <c r="D56" s="59"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="58"/>
-      <c r="J56" s="58"/>
-      <c r="K56" s="58"/>
-      <c r="L56" s="58"/>
-      <c r="M56" s="58"/>
-      <c r="N56" s="58"/>
-      <c r="O56" s="58"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="61"/>
+      <c r="H56" s="61"/>
+      <c r="I56" s="61"/>
+      <c r="J56" s="61"/>
+      <c r="K56" s="61"/>
+      <c r="L56" s="61"/>
+      <c r="M56" s="61"/>
+      <c r="N56" s="61"/>
+      <c r="O56" s="61"/>
     </row>
     <row r="57" spans="3:15" ht="14" customHeight="1">
-      <c r="C57" s="59"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="58"/>
-      <c r="L57" s="58"/>
-      <c r="M57" s="58"/>
-      <c r="N57" s="58"/>
-      <c r="O57" s="58"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="61"/>
+      <c r="H57" s="61"/>
+      <c r="I57" s="61"/>
+      <c r="J57" s="61"/>
+      <c r="K57" s="61"/>
+      <c r="L57" s="61"/>
+      <c r="M57" s="61"/>
+      <c r="N57" s="61"/>
+      <c r="O57" s="61"/>
     </row>
     <row r="58" spans="3:15" ht="14" customHeight="1">
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
-      <c r="J58" s="58"/>
-      <c r="K58" s="58"/>
-      <c r="L58" s="58"/>
-      <c r="M58" s="58"/>
-      <c r="N58" s="58"/>
-      <c r="O58" s="58"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="61"/>
+      <c r="K58" s="61"/>
+      <c r="L58" s="61"/>
+      <c r="M58" s="61"/>
+      <c r="N58" s="61"/>
+      <c r="O58" s="61"/>
     </row>
     <row r="59" spans="3:15" ht="14" customHeight="1">
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="57"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="58"/>
-      <c r="M59" s="58"/>
-      <c r="N59" s="58"/>
-      <c r="O59" s="58"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="61"/>
+      <c r="H59" s="61"/>
+      <c r="I59" s="61"/>
+      <c r="J59" s="61"/>
+      <c r="K59" s="61"/>
+      <c r="L59" s="61"/>
+      <c r="M59" s="61"/>
+      <c r="N59" s="61"/>
+      <c r="O59" s="61"/>
     </row>
     <row r="60" spans="3:15" ht="14" customHeight="1">
-      <c r="C60" s="59"/>
-      <c r="D60" s="59"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="58"/>
-      <c r="K60" s="58"/>
-      <c r="L60" s="58"/>
-      <c r="M60" s="58"/>
-      <c r="N60" s="58"/>
-      <c r="O60" s="58"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="61"/>
+      <c r="H60" s="61"/>
+      <c r="I60" s="61"/>
+      <c r="J60" s="61"/>
+      <c r="K60" s="61"/>
+      <c r="L60" s="61"/>
+      <c r="M60" s="61"/>
+      <c r="N60" s="61"/>
+      <c r="O60" s="61"/>
     </row>
     <row r="61" spans="3:15" ht="14" customHeight="1">
-      <c r="C61" s="59"/>
-      <c r="D61" s="59"/>
-      <c r="E61" s="59"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="58"/>
-      <c r="K61" s="58"/>
-      <c r="L61" s="58"/>
-      <c r="M61" s="58"/>
-      <c r="N61" s="58"/>
-      <c r="O61" s="58"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="52"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="61"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="61"/>
+      <c r="J61" s="61"/>
+      <c r="K61" s="61"/>
+      <c r="L61" s="61"/>
+      <c r="M61" s="61"/>
+      <c r="N61" s="61"/>
+      <c r="O61" s="61"/>
     </row>
     <row r="62" spans="3:15" ht="14" customHeight="1">
-      <c r="C62" s="59"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="59"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="58"/>
-      <c r="I62" s="58"/>
-      <c r="J62" s="58"/>
-      <c r="K62" s="58"/>
-      <c r="L62" s="58"/>
-      <c r="M62" s="58"/>
-      <c r="N62" s="58"/>
-      <c r="O62" s="58"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="61"/>
+      <c r="K62" s="61"/>
+      <c r="L62" s="61"/>
+      <c r="M62" s="61"/>
+      <c r="N62" s="61"/>
+      <c r="O62" s="61"/>
     </row>
     <row r="63" spans="3:15" ht="14" customHeight="1">
-      <c r="C63" s="59"/>
-      <c r="D63" s="59"/>
-      <c r="E63" s="59"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="58"/>
-      <c r="K63" s="58"/>
-      <c r="L63" s="58"/>
-      <c r="M63" s="58"/>
-      <c r="N63" s="58"/>
-      <c r="O63" s="58"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="G63" s="61"/>
+      <c r="H63" s="61"/>
+      <c r="I63" s="61"/>
+      <c r="J63" s="61"/>
+      <c r="K63" s="61"/>
+      <c r="L63" s="61"/>
+      <c r="M63" s="61"/>
+      <c r="N63" s="61"/>
+      <c r="O63" s="61"/>
     </row>
     <row r="64" spans="3:15" ht="14" customHeight="1">
-      <c r="C64" s="59"/>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="58"/>
-      <c r="I64" s="58"/>
-      <c r="J64" s="58"/>
-      <c r="K64" s="58"/>
-      <c r="L64" s="58"/>
-      <c r="M64" s="58"/>
-      <c r="N64" s="58"/>
-      <c r="O64" s="58"/>
+      <c r="C64" s="52"/>
+      <c r="D64" s="52"/>
+      <c r="E64" s="52"/>
+      <c r="G64" s="61"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="61"/>
+      <c r="K64" s="61"/>
+      <c r="L64" s="61"/>
+      <c r="M64" s="61"/>
+      <c r="N64" s="61"/>
+      <c r="O64" s="61"/>
     </row>
     <row r="65" spans="3:15" ht="14" customHeight="1">
-      <c r="C65" s="59"/>
-      <c r="D65" s="59"/>
-      <c r="E65" s="59"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58"/>
-      <c r="I65" s="58"/>
-      <c r="J65" s="58"/>
-      <c r="K65" s="58"/>
-      <c r="L65" s="58"/>
-      <c r="M65" s="58"/>
-      <c r="N65" s="58"/>
-      <c r="O65" s="58"/>
+      <c r="C65" s="52"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="52"/>
+      <c r="G65" s="61"/>
+      <c r="H65" s="61"/>
+      <c r="I65" s="61"/>
+      <c r="J65" s="61"/>
+      <c r="K65" s="61"/>
+      <c r="L65" s="61"/>
+      <c r="M65" s="61"/>
+      <c r="N65" s="61"/>
+      <c r="O65" s="61"/>
     </row>
     <row r="66" spans="3:15" ht="14" customHeight="1">
-      <c r="C66" s="59"/>
-      <c r="D66" s="59"/>
-      <c r="E66" s="59"/>
-      <c r="G66" s="58"/>
-      <c r="H66" s="58"/>
-      <c r="I66" s="58"/>
-      <c r="J66" s="58"/>
-      <c r="K66" s="58"/>
-      <c r="L66" s="58"/>
-      <c r="M66" s="58"/>
-      <c r="N66" s="58"/>
-      <c r="O66" s="58"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="52"/>
+      <c r="G66" s="61"/>
+      <c r="H66" s="61"/>
+      <c r="I66" s="61"/>
+      <c r="J66" s="61"/>
+      <c r="K66" s="61"/>
+      <c r="L66" s="61"/>
+      <c r="M66" s="61"/>
+      <c r="N66" s="61"/>
+      <c r="O66" s="61"/>
     </row>
     <row r="67" spans="3:15" ht="14" customHeight="1">
-      <c r="C67" s="59"/>
-      <c r="D67" s="59"/>
-      <c r="E67" s="59"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58"/>
-      <c r="I67" s="58"/>
-      <c r="J67" s="58"/>
-      <c r="K67" s="58"/>
-      <c r="L67" s="58"/>
-      <c r="M67" s="58"/>
-      <c r="N67" s="58"/>
-      <c r="O67" s="58"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="52"/>
+      <c r="G67" s="61"/>
+      <c r="H67" s="61"/>
+      <c r="I67" s="61"/>
+      <c r="J67" s="61"/>
+      <c r="K67" s="61"/>
+      <c r="L67" s="61"/>
+      <c r="M67" s="61"/>
+      <c r="N67" s="61"/>
+      <c r="O67" s="61"/>
     </row>
     <row r="68" spans="3:15" ht="14" customHeight="1">
-      <c r="C68" s="59"/>
-      <c r="D68" s="59"/>
-      <c r="E68" s="59"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
-      <c r="J68" s="58"/>
-      <c r="K68" s="58"/>
-      <c r="L68" s="58"/>
-      <c r="M68" s="58"/>
-      <c r="N68" s="58"/>
-      <c r="O68" s="58"/>
+      <c r="C68" s="52"/>
+      <c r="D68" s="52"/>
+      <c r="E68" s="52"/>
+      <c r="G68" s="61"/>
+      <c r="H68" s="61"/>
+      <c r="I68" s="61"/>
+      <c r="J68" s="61"/>
+      <c r="K68" s="61"/>
+      <c r="L68" s="61"/>
+      <c r="M68" s="61"/>
+      <c r="N68" s="61"/>
+      <c r="O68" s="61"/>
     </row>
     <row r="69" spans="3:15" ht="14" customHeight="1">
-      <c r="C69" s="59"/>
-      <c r="D69" s="59"/>
-      <c r="E69" s="59"/>
-      <c r="G69" s="58"/>
-      <c r="H69" s="58"/>
-      <c r="I69" s="58"/>
-      <c r="J69" s="58"/>
-      <c r="K69" s="58"/>
-      <c r="L69" s="58"/>
-      <c r="M69" s="58"/>
-      <c r="N69" s="58"/>
-      <c r="O69" s="58"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="52"/>
+      <c r="G69" s="61"/>
+      <c r="H69" s="61"/>
+      <c r="I69" s="61"/>
+      <c r="J69" s="61"/>
+      <c r="K69" s="61"/>
+      <c r="L69" s="61"/>
+      <c r="M69" s="61"/>
+      <c r="N69" s="61"/>
+      <c r="O69" s="61"/>
     </row>
     <row r="70" spans="3:15" ht="14" customHeight="1">
-      <c r="C70" s="59"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="59"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
-      <c r="I70" s="58"/>
-      <c r="J70" s="58"/>
-      <c r="K70" s="58"/>
-      <c r="L70" s="58"/>
-      <c r="M70" s="58"/>
-      <c r="N70" s="58"/>
-      <c r="O70" s="58"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="G70" s="61"/>
+      <c r="H70" s="61"/>
+      <c r="I70" s="61"/>
+      <c r="J70" s="61"/>
+      <c r="K70" s="61"/>
+      <c r="L70" s="61"/>
+      <c r="M70" s="61"/>
+      <c r="N70" s="61"/>
+      <c r="O70" s="61"/>
     </row>
     <row r="71" spans="3:15" ht="14" customHeight="1">
-      <c r="C71" s="59"/>
-      <c r="D71" s="59"/>
-      <c r="E71" s="59"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="58"/>
-      <c r="I71" s="58"/>
-      <c r="J71" s="58"/>
-      <c r="K71" s="58"/>
-      <c r="L71" s="58"/>
-      <c r="M71" s="58"/>
-      <c r="N71" s="58"/>
-      <c r="O71" s="58"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="52"/>
+      <c r="E71" s="52"/>
+      <c r="G71" s="61"/>
+      <c r="H71" s="61"/>
+      <c r="I71" s="61"/>
+      <c r="J71" s="61"/>
+      <c r="K71" s="61"/>
+      <c r="L71" s="61"/>
+      <c r="M71" s="61"/>
+      <c r="N71" s="61"/>
+      <c r="O71" s="61"/>
     </row>
     <row r="72" spans="3:15" ht="14" customHeight="1">
-      <c r="C72" s="59"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="59"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
-      <c r="J72" s="58"/>
-      <c r="K72" s="58"/>
-      <c r="L72" s="58"/>
-      <c r="M72" s="58"/>
-      <c r="N72" s="58"/>
-      <c r="O72" s="58"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52"/>
+      <c r="E72" s="52"/>
+      <c r="G72" s="61"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="61"/>
+      <c r="J72" s="61"/>
+      <c r="K72" s="61"/>
+      <c r="L72" s="61"/>
+      <c r="M72" s="61"/>
+      <c r="N72" s="61"/>
+      <c r="O72" s="61"/>
     </row>
     <row r="73" spans="3:15" ht="14" customHeight="1">
-      <c r="C73" s="59"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="59"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="58"/>
-      <c r="I73" s="58"/>
-      <c r="J73" s="58"/>
-      <c r="K73" s="58"/>
-      <c r="L73" s="58"/>
-      <c r="M73" s="58"/>
-      <c r="N73" s="58"/>
-      <c r="O73" s="58"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="G73" s="61"/>
+      <c r="H73" s="61"/>
+      <c r="I73" s="61"/>
+      <c r="J73" s="61"/>
+      <c r="K73" s="61"/>
+      <c r="L73" s="61"/>
+      <c r="M73" s="61"/>
+      <c r="N73" s="61"/>
+      <c r="O73" s="61"/>
     </row>
     <row r="74" spans="3:15" ht="14" customHeight="1">
-      <c r="C74" s="59"/>
-      <c r="D74" s="59"/>
-      <c r="E74" s="59"/>
-      <c r="G74" s="60"/>
-      <c r="H74" s="60"/>
-      <c r="I74" s="60"/>
-      <c r="J74" s="60"/>
-      <c r="K74" s="60"/>
-      <c r="L74" s="60"/>
-      <c r="M74" s="60"/>
-      <c r="N74" s="60"/>
-      <c r="O74" s="60"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="52"/>
+      <c r="E74" s="52"/>
+      <c r="G74" s="53"/>
+      <c r="H74" s="53"/>
+      <c r="I74" s="53"/>
+      <c r="J74" s="53"/>
+      <c r="K74" s="53"/>
+      <c r="L74" s="53"/>
+      <c r="M74" s="53"/>
+      <c r="N74" s="53"/>
+      <c r="O74" s="53"/>
     </row>
     <row r="75" spans="3:15" ht="14" customHeight="1">
-      <c r="C75" s="59"/>
-      <c r="D75" s="59"/>
-      <c r="E75" s="59"/>
-      <c r="G75" s="60"/>
-      <c r="H75" s="60"/>
-      <c r="I75" s="60"/>
-      <c r="J75" s="60"/>
-      <c r="K75" s="60"/>
-      <c r="L75" s="60"/>
-      <c r="M75" s="60"/>
-      <c r="N75" s="60"/>
-      <c r="O75" s="60"/>
+      <c r="C75" s="52"/>
+      <c r="D75" s="52"/>
+      <c r="E75" s="52"/>
+      <c r="G75" s="53"/>
+      <c r="H75" s="53"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
+      <c r="L75" s="53"/>
+      <c r="M75" s="53"/>
+      <c r="N75" s="53"/>
+      <c r="O75" s="53"/>
     </row>
     <row r="76" spans="3:15" ht="14" customHeight="1">
-      <c r="C76" s="59"/>
-      <c r="D76" s="59"/>
-      <c r="E76" s="59"/>
-      <c r="G76" s="60"/>
-      <c r="H76" s="60"/>
-      <c r="I76" s="60"/>
-      <c r="J76" s="60"/>
-      <c r="K76" s="60"/>
-      <c r="L76" s="60"/>
-      <c r="M76" s="60"/>
-      <c r="N76" s="60"/>
-      <c r="O76" s="60"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="52"/>
+      <c r="E76" s="52"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="53"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="53"/>
+      <c r="K76" s="53"/>
+      <c r="L76" s="53"/>
+      <c r="M76" s="53"/>
+      <c r="N76" s="53"/>
+      <c r="O76" s="53"/>
     </row>
     <row r="77" spans="3:15" ht="14" customHeight="1">
-      <c r="C77" s="59"/>
-      <c r="D77" s="59"/>
-      <c r="E77" s="59"/>
-      <c r="G77" s="60"/>
-      <c r="H77" s="60"/>
-      <c r="I77" s="60"/>
-      <c r="J77" s="60"/>
-      <c r="K77" s="60"/>
-      <c r="L77" s="60"/>
-      <c r="M77" s="60"/>
-      <c r="N77" s="60"/>
-      <c r="O77" s="60"/>
+      <c r="C77" s="52"/>
+      <c r="D77" s="52"/>
+      <c r="E77" s="52"/>
+      <c r="G77" s="53"/>
+      <c r="H77" s="53"/>
+      <c r="I77" s="53"/>
+      <c r="J77" s="53"/>
+      <c r="K77" s="53"/>
+      <c r="L77" s="53"/>
+      <c r="M77" s="53"/>
+      <c r="N77" s="53"/>
+      <c r="O77" s="53"/>
     </row>
     <row r="78" spans="3:15" ht="14" customHeight="1">
-      <c r="C78" s="59"/>
-      <c r="D78" s="59"/>
-      <c r="E78" s="59"/>
-      <c r="G78" s="60"/>
-      <c r="H78" s="60"/>
-      <c r="I78" s="60"/>
-      <c r="J78" s="60"/>
-      <c r="K78" s="60"/>
-      <c r="L78" s="60"/>
-      <c r="M78" s="60"/>
-      <c r="N78" s="60"/>
-      <c r="O78" s="60"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="52"/>
+      <c r="E78" s="52"/>
+      <c r="G78" s="53"/>
+      <c r="H78" s="53"/>
+      <c r="I78" s="53"/>
+      <c r="J78" s="53"/>
+      <c r="K78" s="53"/>
+      <c r="L78" s="53"/>
+      <c r="M78" s="53"/>
+      <c r="N78" s="53"/>
+      <c r="O78" s="53"/>
     </row>
     <row r="79" spans="3:15" ht="14" customHeight="1">
-      <c r="C79" s="59"/>
-      <c r="D79" s="59"/>
-      <c r="E79" s="59"/>
-      <c r="G79" s="60"/>
-      <c r="H79" s="60"/>
-      <c r="I79" s="60"/>
-      <c r="J79" s="60"/>
-      <c r="K79" s="60"/>
-      <c r="L79" s="60"/>
-      <c r="M79" s="60"/>
-      <c r="N79" s="60"/>
-      <c r="O79" s="60"/>
+      <c r="C79" s="52"/>
+      <c r="D79" s="52"/>
+      <c r="E79" s="52"/>
+      <c r="G79" s="53"/>
+      <c r="H79" s="53"/>
+      <c r="I79" s="53"/>
+      <c r="J79" s="53"/>
+      <c r="K79" s="53"/>
+      <c r="L79" s="53"/>
+      <c r="M79" s="53"/>
+      <c r="N79" s="53"/>
+      <c r="O79" s="53"/>
     </row>
     <row r="80" spans="3:15" ht="14" customHeight="1">
-      <c r="C80" s="59"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="59"/>
-      <c r="G80" s="60"/>
-      <c r="H80" s="60"/>
-      <c r="I80" s="60"/>
-      <c r="J80" s="60"/>
-      <c r="K80" s="60"/>
-      <c r="L80" s="60"/>
-      <c r="M80" s="60"/>
-      <c r="N80" s="60"/>
-      <c r="O80" s="60"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="52"/>
+      <c r="E80" s="52"/>
+      <c r="G80" s="53"/>
+      <c r="H80" s="53"/>
+      <c r="I80" s="53"/>
+      <c r="J80" s="53"/>
+      <c r="K80" s="53"/>
+      <c r="L80" s="53"/>
+      <c r="M80" s="53"/>
+      <c r="N80" s="53"/>
+      <c r="O80" s="53"/>
     </row>
     <row r="81" spans="3:15" ht="14" customHeight="1">
-      <c r="C81" s="59"/>
-      <c r="D81" s="59"/>
-      <c r="E81" s="59"/>
-      <c r="G81" s="60"/>
-      <c r="H81" s="60"/>
-      <c r="I81" s="60"/>
-      <c r="J81" s="60"/>
-      <c r="K81" s="60"/>
-      <c r="L81" s="60"/>
-      <c r="M81" s="60"/>
-      <c r="N81" s="60"/>
-      <c r="O81" s="60"/>
+      <c r="C81" s="52"/>
+      <c r="D81" s="52"/>
+      <c r="E81" s="52"/>
+      <c r="G81" s="53"/>
+      <c r="H81" s="53"/>
+      <c r="I81" s="53"/>
+      <c r="J81" s="53"/>
+      <c r="K81" s="53"/>
+      <c r="L81" s="53"/>
+      <c r="M81" s="53"/>
+      <c r="N81" s="53"/>
+      <c r="O81" s="53"/>
     </row>
     <row r="82" spans="3:15" ht="14" customHeight="1">
-      <c r="C82" s="59"/>
-      <c r="D82" s="59"/>
-      <c r="E82" s="59"/>
-      <c r="G82" s="60"/>
-      <c r="H82" s="60"/>
-      <c r="I82" s="60"/>
-      <c r="J82" s="60"/>
-      <c r="K82" s="60"/>
-      <c r="L82" s="60"/>
-      <c r="M82" s="60"/>
-      <c r="N82" s="60"/>
-      <c r="O82" s="60"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="52"/>
+      <c r="E82" s="52"/>
+      <c r="G82" s="53"/>
+      <c r="H82" s="53"/>
+      <c r="I82" s="53"/>
+      <c r="J82" s="53"/>
+      <c r="K82" s="53"/>
+      <c r="L82" s="53"/>
+      <c r="M82" s="53"/>
+      <c r="N82" s="53"/>
+      <c r="O82" s="53"/>
     </row>
     <row r="83" spans="3:15" ht="14" customHeight="1">
-      <c r="C83" s="59"/>
-      <c r="D83" s="59"/>
-      <c r="E83" s="59"/>
-      <c r="G83" s="60"/>
-      <c r="H83" s="60"/>
-      <c r="I83" s="60"/>
-      <c r="J83" s="60"/>
-      <c r="K83" s="60"/>
-      <c r="L83" s="60"/>
-      <c r="M83" s="60"/>
-      <c r="N83" s="60"/>
-      <c r="O83" s="60"/>
+      <c r="C83" s="52"/>
+      <c r="D83" s="52"/>
+      <c r="E83" s="52"/>
+      <c r="G83" s="53"/>
+      <c r="H83" s="53"/>
+      <c r="I83" s="53"/>
+      <c r="J83" s="53"/>
+      <c r="K83" s="53"/>
+      <c r="L83" s="53"/>
+      <c r="M83" s="53"/>
+      <c r="N83" s="53"/>
+      <c r="O83" s="53"/>
     </row>
     <row r="84" spans="3:15" ht="14" customHeight="1">
-      <c r="C84" s="59"/>
-      <c r="D84" s="59"/>
-      <c r="E84" s="59"/>
-      <c r="G84" s="60"/>
-      <c r="H84" s="60"/>
-      <c r="I84" s="60"/>
-      <c r="J84" s="60"/>
-      <c r="K84" s="60"/>
-      <c r="L84" s="60"/>
-      <c r="M84" s="60"/>
-      <c r="N84" s="60"/>
-      <c r="O84" s="60"/>
+      <c r="C84" s="52"/>
+      <c r="D84" s="52"/>
+      <c r="E84" s="52"/>
+      <c r="G84" s="53"/>
+      <c r="H84" s="53"/>
+      <c r="I84" s="53"/>
+      <c r="J84" s="53"/>
+      <c r="K84" s="53"/>
+      <c r="L84" s="53"/>
+      <c r="M84" s="53"/>
+      <c r="N84" s="53"/>
+      <c r="O84" s="53"/>
     </row>
     <row r="85" spans="3:15" ht="14" customHeight="1">
-      <c r="C85" s="59"/>
-      <c r="D85" s="59"/>
-      <c r="E85" s="59"/>
-      <c r="G85" s="60"/>
-      <c r="H85" s="60"/>
-      <c r="I85" s="60"/>
-      <c r="J85" s="60"/>
-      <c r="K85" s="60"/>
-      <c r="L85" s="60"/>
-      <c r="M85" s="60"/>
-      <c r="N85" s="60"/>
-      <c r="O85" s="60"/>
+      <c r="C85" s="52"/>
+      <c r="D85" s="52"/>
+      <c r="E85" s="52"/>
+      <c r="G85" s="53"/>
+      <c r="H85" s="53"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="53"/>
+      <c r="K85" s="53"/>
+      <c r="L85" s="53"/>
+      <c r="M85" s="53"/>
+      <c r="N85" s="53"/>
+      <c r="O85" s="53"/>
     </row>
     <row r="86" spans="3:15" ht="14" customHeight="1">
-      <c r="C86" s="59"/>
-      <c r="D86" s="59"/>
-      <c r="E86" s="59"/>
-      <c r="G86" s="60"/>
-      <c r="H86" s="60"/>
-      <c r="I86" s="60"/>
-      <c r="J86" s="60"/>
-      <c r="K86" s="60"/>
-      <c r="L86" s="60"/>
-      <c r="M86" s="60"/>
-      <c r="N86" s="60"/>
-      <c r="O86" s="60"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="G86" s="53"/>
+      <c r="H86" s="53"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="53"/>
+      <c r="K86" s="53"/>
+      <c r="L86" s="53"/>
+      <c r="M86" s="53"/>
+      <c r="N86" s="53"/>
+      <c r="O86" s="53"/>
     </row>
     <row r="87" spans="3:15" ht="14" customHeight="1">
-      <c r="C87" s="59"/>
-      <c r="D87" s="59"/>
-      <c r="E87" s="59"/>
-      <c r="G87" s="60"/>
-      <c r="H87" s="60"/>
-      <c r="I87" s="60"/>
-      <c r="J87" s="60"/>
-      <c r="K87" s="60"/>
-      <c r="L87" s="60"/>
-      <c r="M87" s="60"/>
-      <c r="N87" s="60"/>
-      <c r="O87" s="60"/>
+      <c r="C87" s="52"/>
+      <c r="D87" s="52"/>
+      <c r="E87" s="52"/>
+      <c r="G87" s="53"/>
+      <c r="H87" s="53"/>
+      <c r="I87" s="53"/>
+      <c r="J87" s="53"/>
+      <c r="K87" s="53"/>
+      <c r="L87" s="53"/>
+      <c r="M87" s="53"/>
+      <c r="N87" s="53"/>
+      <c r="O87" s="53"/>
     </row>
     <row r="88" spans="3:15" ht="14" customHeight="1">
-      <c r="C88" s="59"/>
-      <c r="D88" s="59"/>
-      <c r="E88" s="59"/>
-      <c r="G88" s="60"/>
-      <c r="H88" s="60"/>
-      <c r="I88" s="60"/>
-      <c r="J88" s="60"/>
-      <c r="K88" s="60"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="60"/>
-      <c r="N88" s="60"/>
-      <c r="O88" s="60"/>
+      <c r="C88" s="52"/>
+      <c r="D88" s="52"/>
+      <c r="E88" s="52"/>
+      <c r="G88" s="53"/>
+      <c r="H88" s="53"/>
+      <c r="I88" s="53"/>
+      <c r="J88" s="53"/>
+      <c r="K88" s="53"/>
+      <c r="L88" s="53"/>
+      <c r="M88" s="53"/>
+      <c r="N88" s="53"/>
+      <c r="O88" s="53"/>
     </row>
     <row r="89" spans="3:15" ht="14" customHeight="1">
-      <c r="C89" s="59"/>
-      <c r="D89" s="59"/>
-      <c r="E89" s="59"/>
-      <c r="G89" s="60"/>
-      <c r="H89" s="60"/>
-      <c r="I89" s="60"/>
-      <c r="J89" s="60"/>
-      <c r="K89" s="60"/>
-      <c r="L89" s="60"/>
-      <c r="M89" s="60"/>
-      <c r="N89" s="60"/>
-      <c r="O89" s="60"/>
+      <c r="C89" s="52"/>
+      <c r="D89" s="52"/>
+      <c r="E89" s="52"/>
+      <c r="G89" s="53"/>
+      <c r="H89" s="53"/>
+      <c r="I89" s="53"/>
+      <c r="J89" s="53"/>
+      <c r="K89" s="53"/>
+      <c r="L89" s="53"/>
+      <c r="M89" s="53"/>
+      <c r="N89" s="53"/>
+      <c r="O89" s="53"/>
     </row>
     <row r="90" spans="3:15" ht="14" customHeight="1">
-      <c r="C90" s="59"/>
-      <c r="D90" s="59"/>
-      <c r="E90" s="59"/>
-      <c r="G90" s="60"/>
-      <c r="H90" s="60"/>
-      <c r="I90" s="60"/>
-      <c r="J90" s="60"/>
-      <c r="K90" s="60"/>
-      <c r="L90" s="60"/>
-      <c r="M90" s="60"/>
-      <c r="N90" s="60"/>
-      <c r="O90" s="60"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="52"/>
+      <c r="E90" s="52"/>
+      <c r="G90" s="53"/>
+      <c r="H90" s="53"/>
+      <c r="I90" s="53"/>
+      <c r="J90" s="53"/>
+      <c r="K90" s="53"/>
+      <c r="L90" s="53"/>
+      <c r="M90" s="53"/>
+      <c r="N90" s="53"/>
+      <c r="O90" s="53"/>
     </row>
     <row r="91" spans="3:15" ht="14" customHeight="1">
-      <c r="C91" s="59"/>
-      <c r="D91" s="59"/>
-      <c r="E91" s="59"/>
-      <c r="G91" s="60"/>
-      <c r="H91" s="60"/>
-      <c r="I91" s="60"/>
-      <c r="J91" s="60"/>
-      <c r="K91" s="60"/>
-      <c r="L91" s="60"/>
-      <c r="M91" s="60"/>
-      <c r="N91" s="60"/>
-      <c r="O91" s="60"/>
+      <c r="C91" s="52"/>
+      <c r="D91" s="52"/>
+      <c r="E91" s="52"/>
+      <c r="G91" s="53"/>
+      <c r="H91" s="53"/>
+      <c r="I91" s="53"/>
+      <c r="J91" s="53"/>
+      <c r="K91" s="53"/>
+      <c r="L91" s="53"/>
+      <c r="M91" s="53"/>
+      <c r="N91" s="53"/>
+      <c r="O91" s="53"/>
     </row>
     <row r="92" spans="3:15" ht="14" customHeight="1">
-      <c r="C92" s="59"/>
-      <c r="D92" s="59"/>
-      <c r="E92" s="59"/>
-      <c r="G92" s="60"/>
-      <c r="H92" s="60"/>
-      <c r="I92" s="60"/>
-      <c r="J92" s="60"/>
-      <c r="K92" s="60"/>
-      <c r="L92" s="60"/>
-      <c r="M92" s="60"/>
-      <c r="N92" s="60"/>
-      <c r="O92" s="60"/>
+      <c r="C92" s="52"/>
+      <c r="D92" s="52"/>
+      <c r="E92" s="52"/>
+      <c r="G92" s="53"/>
+      <c r="H92" s="53"/>
+      <c r="I92" s="53"/>
+      <c r="J92" s="53"/>
+      <c r="K92" s="53"/>
+      <c r="L92" s="53"/>
+      <c r="M92" s="53"/>
+      <c r="N92" s="53"/>
+      <c r="O92" s="53"/>
     </row>
     <row r="93" spans="3:15" ht="14" customHeight="1">
-      <c r="C93" s="59"/>
-      <c r="D93" s="59"/>
-      <c r="E93" s="59"/>
-      <c r="G93" s="60"/>
-      <c r="H93" s="60"/>
-      <c r="I93" s="60"/>
-      <c r="J93" s="60"/>
-      <c r="K93" s="60"/>
-      <c r="L93" s="60"/>
-      <c r="M93" s="60"/>
-      <c r="N93" s="60"/>
-      <c r="O93" s="60"/>
+      <c r="C93" s="52"/>
+      <c r="D93" s="52"/>
+      <c r="E93" s="52"/>
+      <c r="G93" s="53"/>
+      <c r="H93" s="53"/>
+      <c r="I93" s="53"/>
+      <c r="J93" s="53"/>
+      <c r="K93" s="53"/>
+      <c r="L93" s="53"/>
+      <c r="M93" s="53"/>
+      <c r="N93" s="53"/>
+      <c r="O93" s="53"/>
     </row>
     <row r="94" spans="3:15" ht="14" customHeight="1">
-      <c r="C94" s="59"/>
-      <c r="D94" s="59"/>
-      <c r="E94" s="59"/>
-      <c r="G94" s="60"/>
-      <c r="H94" s="60"/>
-      <c r="I94" s="60"/>
-      <c r="J94" s="60"/>
-      <c r="K94" s="60"/>
-      <c r="L94" s="60"/>
-      <c r="M94" s="60"/>
-      <c r="N94" s="60"/>
-      <c r="O94" s="60"/>
+      <c r="C94" s="52"/>
+      <c r="D94" s="52"/>
+      <c r="E94" s="52"/>
+      <c r="G94" s="53"/>
+      <c r="H94" s="53"/>
+      <c r="I94" s="53"/>
+      <c r="J94" s="53"/>
+      <c r="K94" s="53"/>
+      <c r="L94" s="53"/>
+      <c r="M94" s="53"/>
+      <c r="N94" s="53"/>
+      <c r="O94" s="53"/>
     </row>
     <row r="95" spans="3:15" ht="14" customHeight="1">
-      <c r="C95" s="59"/>
-      <c r="D95" s="59"/>
-      <c r="E95" s="59"/>
-      <c r="G95" s="60"/>
-      <c r="H95" s="60"/>
-      <c r="I95" s="60"/>
-      <c r="J95" s="60"/>
-      <c r="K95" s="60"/>
-      <c r="L95" s="60"/>
-      <c r="M95" s="60"/>
-      <c r="N95" s="60"/>
-      <c r="O95" s="60"/>
+      <c r="C95" s="52"/>
+      <c r="D95" s="52"/>
+      <c r="E95" s="52"/>
+      <c r="G95" s="53"/>
+      <c r="H95" s="53"/>
+      <c r="I95" s="53"/>
+      <c r="J95" s="53"/>
+      <c r="K95" s="53"/>
+      <c r="L95" s="53"/>
+      <c r="M95" s="53"/>
+      <c r="N95" s="53"/>
+      <c r="O95" s="53"/>
     </row>
     <row r="96" spans="3:15" ht="14" customHeight="1">
-      <c r="C96" s="59"/>
-      <c r="D96" s="59"/>
-      <c r="E96" s="59"/>
-      <c r="G96" s="60"/>
-      <c r="H96" s="60"/>
-      <c r="I96" s="60"/>
-      <c r="J96" s="60"/>
-      <c r="K96" s="60"/>
-      <c r="L96" s="60"/>
-      <c r="M96" s="60"/>
-      <c r="N96" s="60"/>
-      <c r="O96" s="60"/>
+      <c r="C96" s="52"/>
+      <c r="D96" s="52"/>
+      <c r="E96" s="52"/>
+      <c r="G96" s="53"/>
+      <c r="H96" s="53"/>
+      <c r="I96" s="53"/>
+      <c r="J96" s="53"/>
+      <c r="K96" s="53"/>
+      <c r="L96" s="53"/>
+      <c r="M96" s="53"/>
+      <c r="N96" s="53"/>
+      <c r="O96" s="53"/>
     </row>
     <row r="97" spans="2:15" ht="14" customHeight="1">
-      <c r="C97" s="59"/>
-      <c r="D97" s="59"/>
-      <c r="E97" s="59"/>
-      <c r="G97" s="60"/>
-      <c r="H97" s="60"/>
-      <c r="I97" s="60"/>
-      <c r="J97" s="60"/>
-      <c r="K97" s="60"/>
-      <c r="L97" s="60"/>
-      <c r="M97" s="60"/>
-      <c r="N97" s="60"/>
-      <c r="O97" s="60"/>
+      <c r="C97" s="52"/>
+      <c r="D97" s="52"/>
+      <c r="E97" s="52"/>
+      <c r="G97" s="53"/>
+      <c r="H97" s="53"/>
+      <c r="I97" s="53"/>
+      <c r="J97" s="53"/>
+      <c r="K97" s="53"/>
+      <c r="L97" s="53"/>
+      <c r="M97" s="53"/>
+      <c r="N97" s="53"/>
+      <c r="O97" s="53"/>
     </row>
     <row r="98" spans="2:15" ht="14" customHeight="1">
-      <c r="C98" s="59"/>
-      <c r="D98" s="59"/>
-      <c r="E98" s="59"/>
-      <c r="G98" s="60"/>
-      <c r="H98" s="60"/>
-      <c r="I98" s="60"/>
-      <c r="J98" s="60"/>
-      <c r="K98" s="60"/>
-      <c r="L98" s="60"/>
-      <c r="M98" s="60"/>
-      <c r="N98" s="60"/>
-      <c r="O98" s="60"/>
+      <c r="C98" s="52"/>
+      <c r="D98" s="52"/>
+      <c r="E98" s="52"/>
+      <c r="G98" s="53"/>
+      <c r="H98" s="53"/>
+      <c r="I98" s="53"/>
+      <c r="J98" s="53"/>
+      <c r="K98" s="53"/>
+      <c r="L98" s="53"/>
+      <c r="M98" s="53"/>
+      <c r="N98" s="53"/>
+      <c r="O98" s="53"/>
     </row>
     <row r="99" spans="2:15" ht="14" customHeight="1">
-      <c r="C99" s="59"/>
-      <c r="D99" s="59"/>
-      <c r="E99" s="59"/>
-      <c r="G99" s="60"/>
-      <c r="H99" s="60"/>
-      <c r="I99" s="60"/>
-      <c r="J99" s="60"/>
-      <c r="K99" s="60"/>
-      <c r="L99" s="60"/>
-      <c r="M99" s="60"/>
-      <c r="N99" s="60"/>
-      <c r="O99" s="60"/>
+      <c r="C99" s="52"/>
+      <c r="D99" s="52"/>
+      <c r="E99" s="52"/>
+      <c r="G99" s="53"/>
+      <c r="H99" s="53"/>
+      <c r="I99" s="53"/>
+      <c r="J99" s="53"/>
+      <c r="K99" s="53"/>
+      <c r="L99" s="53"/>
+      <c r="M99" s="53"/>
+      <c r="N99" s="53"/>
+      <c r="O99" s="53"/>
     </row>
     <row r="100" spans="2:15" ht="14" customHeight="1">
-      <c r="C100" s="59"/>
-      <c r="D100" s="59"/>
-      <c r="E100" s="59"/>
-      <c r="G100" s="60"/>
-      <c r="H100" s="60"/>
-      <c r="I100" s="60"/>
-      <c r="J100" s="60"/>
-      <c r="K100" s="60"/>
-      <c r="L100" s="60"/>
-      <c r="M100" s="60"/>
-      <c r="N100" s="60"/>
-      <c r="O100" s="60"/>
+      <c r="C100" s="52"/>
+      <c r="D100" s="52"/>
+      <c r="E100" s="52"/>
+      <c r="G100" s="53"/>
+      <c r="H100" s="53"/>
+      <c r="I100" s="53"/>
+      <c r="J100" s="53"/>
+      <c r="K100" s="53"/>
+      <c r="L100" s="53"/>
+      <c r="M100" s="53"/>
+      <c r="N100" s="53"/>
+      <c r="O100" s="53"/>
     </row>
     <row r="101" spans="2:15" ht="14" customHeight="1">
-      <c r="C101" s="59"/>
-      <c r="D101" s="59"/>
-      <c r="E101" s="59"/>
-      <c r="G101" s="60"/>
-      <c r="H101" s="60"/>
-      <c r="I101" s="60"/>
-      <c r="J101" s="60"/>
-      <c r="K101" s="60"/>
-      <c r="L101" s="60"/>
-      <c r="M101" s="60"/>
-      <c r="N101" s="60"/>
-      <c r="O101" s="60"/>
+      <c r="C101" s="52"/>
+      <c r="D101" s="52"/>
+      <c r="E101" s="52"/>
+      <c r="G101" s="53"/>
+      <c r="H101" s="53"/>
+      <c r="I101" s="53"/>
+      <c r="J101" s="53"/>
+      <c r="K101" s="53"/>
+      <c r="L101" s="53"/>
+      <c r="M101" s="53"/>
+      <c r="N101" s="53"/>
+      <c r="O101" s="53"/>
     </row>
     <row r="102" spans="2:15" ht="14" customHeight="1">
-      <c r="C102" s="61"/>
-      <c r="D102" s="61"/>
-      <c r="E102" s="61"/>
-      <c r="F102" s="61"/>
-      <c r="G102" s="60"/>
-      <c r="H102" s="60"/>
-      <c r="I102" s="60"/>
-      <c r="J102" s="60"/>
-      <c r="K102" s="60"/>
-      <c r="L102" s="60"/>
-      <c r="M102" s="60"/>
-      <c r="N102" s="60"/>
-      <c r="O102" s="60"/>
+      <c r="C102" s="59"/>
+      <c r="D102" s="59"/>
+      <c r="E102" s="59"/>
+      <c r="F102" s="59"/>
+      <c r="G102" s="53"/>
+      <c r="H102" s="53"/>
+      <c r="I102" s="53"/>
+      <c r="J102" s="53"/>
+      <c r="K102" s="53"/>
+      <c r="L102" s="53"/>
+      <c r="M102" s="53"/>
+      <c r="N102" s="53"/>
+      <c r="O102" s="53"/>
     </row>
     <row r="103" spans="2:15" ht="14" customHeight="1">
-      <c r="B103" s="57"/>
-      <c r="C103" s="59"/>
-      <c r="D103" s="59"/>
-      <c r="E103" s="59"/>
-      <c r="F103" s="57"/>
-      <c r="G103" s="60"/>
-      <c r="H103" s="60"/>
-      <c r="I103" s="60"/>
-      <c r="J103" s="60"/>
-      <c r="K103" s="60"/>
-      <c r="L103" s="60"/>
-      <c r="M103" s="60"/>
-      <c r="N103" s="60"/>
-      <c r="O103" s="60"/>
+      <c r="B103" s="51"/>
+      <c r="C103" s="52"/>
+      <c r="D103" s="52"/>
+      <c r="E103" s="52"/>
+      <c r="F103" s="51"/>
+      <c r="G103" s="53"/>
+      <c r="H103" s="53"/>
+      <c r="I103" s="53"/>
+      <c r="J103" s="53"/>
+      <c r="K103" s="53"/>
+      <c r="L103" s="53"/>
+      <c r="M103" s="53"/>
+      <c r="N103" s="53"/>
+      <c r="O103" s="53"/>
     </row>
     <row r="104" spans="2:15" ht="14" customHeight="1">
-      <c r="B104" s="57"/>
-      <c r="C104" s="59"/>
-      <c r="D104" s="59"/>
-      <c r="E104" s="59"/>
-      <c r="F104" s="57"/>
-      <c r="G104" s="60"/>
-      <c r="H104" s="60"/>
-      <c r="I104" s="60"/>
-      <c r="J104" s="60"/>
-      <c r="K104" s="60"/>
-      <c r="L104" s="60"/>
-      <c r="M104" s="60"/>
-      <c r="N104" s="60"/>
-      <c r="O104" s="60"/>
+      <c r="B104" s="51"/>
+      <c r="C104" s="52"/>
+      <c r="D104" s="52"/>
+      <c r="E104" s="52"/>
+      <c r="F104" s="51"/>
+      <c r="G104" s="53"/>
+      <c r="H104" s="53"/>
+      <c r="I104" s="53"/>
+      <c r="J104" s="53"/>
+      <c r="K104" s="53"/>
+      <c r="L104" s="53"/>
+      <c r="M104" s="53"/>
+      <c r="N104" s="53"/>
+      <c r="O104" s="53"/>
     </row>
     <row r="105" spans="2:15" ht="14" customHeight="1">
-      <c r="B105" s="57"/>
-      <c r="C105" s="59"/>
-      <c r="D105" s="59"/>
-      <c r="E105" s="59"/>
-      <c r="F105" s="57"/>
-      <c r="G105" s="60"/>
-      <c r="H105" s="60"/>
-      <c r="I105" s="60"/>
-      <c r="J105" s="60"/>
-      <c r="K105" s="60"/>
-      <c r="L105" s="60"/>
-      <c r="M105" s="60"/>
-      <c r="N105" s="60"/>
-      <c r="O105" s="60"/>
+      <c r="B105" s="51"/>
+      <c r="C105" s="52"/>
+      <c r="D105" s="52"/>
+      <c r="E105" s="52"/>
+      <c r="F105" s="51"/>
+      <c r="G105" s="53"/>
+      <c r="H105" s="53"/>
+      <c r="I105" s="53"/>
+      <c r="J105" s="53"/>
+      <c r="K105" s="53"/>
+      <c r="L105" s="53"/>
+      <c r="M105" s="53"/>
+      <c r="N105" s="53"/>
+      <c r="O105" s="53"/>
     </row>
     <row r="106" spans="2:15" ht="14" customHeight="1">
-      <c r="B106" s="57"/>
-      <c r="C106" s="59"/>
-      <c r="D106" s="59"/>
-      <c r="E106" s="59"/>
-      <c r="F106" s="57"/>
-      <c r="G106" s="60"/>
-      <c r="H106" s="60"/>
-      <c r="I106" s="60"/>
-      <c r="J106" s="60"/>
-      <c r="K106" s="60"/>
-      <c r="L106" s="60"/>
-      <c r="M106" s="60"/>
-      <c r="N106" s="60"/>
-      <c r="O106" s="60"/>
+      <c r="B106" s="51"/>
+      <c r="C106" s="52"/>
+      <c r="D106" s="52"/>
+      <c r="E106" s="52"/>
+      <c r="F106" s="51"/>
+      <c r="G106" s="53"/>
+      <c r="H106" s="53"/>
+      <c r="I106" s="53"/>
+      <c r="J106" s="53"/>
+      <c r="K106" s="53"/>
+      <c r="L106" s="53"/>
+      <c r="M106" s="53"/>
+      <c r="N106" s="53"/>
+      <c r="O106" s="53"/>
     </row>
     <row r="107" spans="2:15" ht="14" customHeight="1">
-      <c r="B107" s="57"/>
-      <c r="C107" s="59"/>
-      <c r="D107" s="59"/>
-      <c r="E107" s="59"/>
-      <c r="F107" s="57"/>
-      <c r="G107" s="60"/>
-      <c r="H107" s="60"/>
-      <c r="I107" s="60"/>
-      <c r="J107" s="60"/>
-      <c r="K107" s="60"/>
-      <c r="L107" s="60"/>
-      <c r="M107" s="60"/>
-      <c r="N107" s="60"/>
-      <c r="O107" s="60"/>
+      <c r="B107" s="51"/>
+      <c r="C107" s="52"/>
+      <c r="D107" s="52"/>
+      <c r="E107" s="52"/>
+      <c r="F107" s="51"/>
+      <c r="G107" s="53"/>
+      <c r="H107" s="53"/>
+      <c r="I107" s="53"/>
+      <c r="J107" s="53"/>
+      <c r="K107" s="53"/>
+      <c r="L107" s="53"/>
+      <c r="M107" s="53"/>
+      <c r="N107" s="53"/>
+      <c r="O107" s="53"/>
     </row>
     <row r="108" spans="2:15" ht="14" customHeight="1">
-      <c r="B108" s="57"/>
-      <c r="C108" s="59"/>
-      <c r="D108" s="59"/>
-      <c r="E108" s="59"/>
-      <c r="F108" s="57"/>
-      <c r="G108" s="60"/>
-      <c r="H108" s="60"/>
-      <c r="I108" s="60"/>
-      <c r="J108" s="60"/>
-      <c r="K108" s="60"/>
-      <c r="L108" s="60"/>
-      <c r="M108" s="60"/>
-      <c r="N108" s="60"/>
-      <c r="O108" s="60"/>
+      <c r="B108" s="51"/>
+      <c r="C108" s="52"/>
+      <c r="D108" s="52"/>
+      <c r="E108" s="52"/>
+      <c r="F108" s="51"/>
+      <c r="G108" s="53"/>
+      <c r="H108" s="53"/>
+      <c r="I108" s="53"/>
+      <c r="J108" s="53"/>
+      <c r="K108" s="53"/>
+      <c r="L108" s="53"/>
+      <c r="M108" s="53"/>
+      <c r="N108" s="53"/>
+      <c r="O108" s="53"/>
     </row>
     <row r="109" spans="2:15" ht="14" customHeight="1">
-      <c r="B109" s="57"/>
-      <c r="C109" s="59"/>
-      <c r="D109" s="59"/>
-      <c r="E109" s="59"/>
-      <c r="F109" s="57"/>
-      <c r="G109" s="60"/>
-      <c r="H109" s="60"/>
-      <c r="I109" s="60"/>
-      <c r="J109" s="60"/>
-      <c r="K109" s="60"/>
-      <c r="L109" s="60"/>
-      <c r="M109" s="60"/>
-      <c r="N109" s="60"/>
-      <c r="O109" s="60"/>
+      <c r="B109" s="51"/>
+      <c r="C109" s="52"/>
+      <c r="D109" s="52"/>
+      <c r="E109" s="52"/>
+      <c r="F109" s="51"/>
+      <c r="G109" s="53"/>
+      <c r="H109" s="53"/>
+      <c r="I109" s="53"/>
+      <c r="J109" s="53"/>
+      <c r="K109" s="53"/>
+      <c r="L109" s="53"/>
+      <c r="M109" s="53"/>
+      <c r="N109" s="53"/>
+      <c r="O109" s="53"/>
     </row>
     <row r="110" spans="2:15" ht="14" customHeight="1">
-      <c r="B110" s="57"/>
-      <c r="C110" s="59"/>
-      <c r="D110" s="59"/>
-      <c r="E110" s="59"/>
-      <c r="F110" s="57"/>
-      <c r="G110" s="60"/>
-      <c r="H110" s="60"/>
-      <c r="I110" s="60"/>
-      <c r="J110" s="60"/>
-      <c r="K110" s="60"/>
-      <c r="L110" s="60"/>
-      <c r="M110" s="60"/>
-      <c r="N110" s="60"/>
-      <c r="O110" s="60"/>
+      <c r="B110" s="51"/>
+      <c r="C110" s="52"/>
+      <c r="D110" s="52"/>
+      <c r="E110" s="52"/>
+      <c r="F110" s="51"/>
+      <c r="G110" s="53"/>
+      <c r="H110" s="53"/>
+      <c r="I110" s="53"/>
+      <c r="J110" s="53"/>
+      <c r="K110" s="53"/>
+      <c r="L110" s="53"/>
+      <c r="M110" s="53"/>
+      <c r="N110" s="53"/>
+      <c r="O110" s="53"/>
     </row>
     <row r="111" spans="2:15" ht="14" customHeight="1">
-      <c r="B111" s="57"/>
-      <c r="C111" s="59"/>
-      <c r="D111" s="59"/>
-      <c r="E111" s="59"/>
-      <c r="F111" s="57"/>
-      <c r="G111" s="60"/>
-      <c r="H111" s="60"/>
-      <c r="I111" s="60"/>
-      <c r="J111" s="60"/>
-      <c r="K111" s="60"/>
-      <c r="L111" s="60"/>
-      <c r="M111" s="60"/>
-      <c r="N111" s="60"/>
-      <c r="O111" s="60"/>
+      <c r="B111" s="51"/>
+      <c r="C111" s="52"/>
+      <c r="D111" s="52"/>
+      <c r="E111" s="52"/>
+      <c r="F111" s="51"/>
+      <c r="G111" s="53"/>
+      <c r="H111" s="53"/>
+      <c r="I111" s="53"/>
+      <c r="J111" s="53"/>
+      <c r="K111" s="53"/>
+      <c r="L111" s="53"/>
+      <c r="M111" s="53"/>
+      <c r="N111" s="53"/>
+      <c r="O111" s="53"/>
     </row>
     <row r="112" spans="2:15" ht="14" customHeight="1">
-      <c r="B112" s="57"/>
-      <c r="C112" s="59"/>
-      <c r="D112" s="59"/>
-      <c r="E112" s="59"/>
-      <c r="F112" s="57"/>
-      <c r="G112" s="60"/>
-      <c r="H112" s="60"/>
-      <c r="I112" s="60"/>
-      <c r="J112" s="60"/>
-      <c r="K112" s="60"/>
-      <c r="L112" s="60"/>
-      <c r="M112" s="60"/>
-      <c r="N112" s="60"/>
-      <c r="O112" s="60"/>
+      <c r="B112" s="51"/>
+      <c r="C112" s="52"/>
+      <c r="D112" s="52"/>
+      <c r="E112" s="52"/>
+      <c r="F112" s="51"/>
+      <c r="G112" s="53"/>
+      <c r="H112" s="53"/>
+      <c r="I112" s="53"/>
+      <c r="J112" s="53"/>
+      <c r="K112" s="53"/>
+      <c r="L112" s="53"/>
+      <c r="M112" s="53"/>
+      <c r="N112" s="53"/>
+      <c r="O112" s="53"/>
     </row>
     <row r="113" spans="2:15" ht="14" customHeight="1">
-      <c r="B113" s="57"/>
-      <c r="C113" s="59"/>
-      <c r="D113" s="59"/>
-      <c r="E113" s="59"/>
-      <c r="F113" s="57"/>
-      <c r="G113" s="60"/>
-      <c r="H113" s="60"/>
-      <c r="I113" s="60"/>
-      <c r="J113" s="60"/>
-      <c r="K113" s="60"/>
-      <c r="L113" s="60"/>
-      <c r="M113" s="60"/>
-      <c r="N113" s="60"/>
-      <c r="O113" s="60"/>
+      <c r="B113" s="51"/>
+      <c r="C113" s="52"/>
+      <c r="D113" s="52"/>
+      <c r="E113" s="52"/>
+      <c r="F113" s="51"/>
+      <c r="G113" s="53"/>
+      <c r="H113" s="53"/>
+      <c r="I113" s="53"/>
+      <c r="J113" s="53"/>
+      <c r="K113" s="53"/>
+      <c r="L113" s="53"/>
+      <c r="M113" s="53"/>
+      <c r="N113" s="53"/>
+      <c r="O113" s="53"/>
     </row>
     <row r="114" spans="2:15" ht="14" customHeight="1">
-      <c r="B114" s="57"/>
-      <c r="C114" s="59"/>
-      <c r="D114" s="59"/>
-      <c r="E114" s="59"/>
-      <c r="F114" s="57"/>
-      <c r="G114" s="60"/>
-      <c r="H114" s="60"/>
-      <c r="I114" s="60"/>
-      <c r="J114" s="60"/>
-      <c r="K114" s="60"/>
-      <c r="L114" s="60"/>
-      <c r="M114" s="60"/>
-      <c r="N114" s="60"/>
-      <c r="O114" s="60"/>
+      <c r="B114" s="51"/>
+      <c r="C114" s="52"/>
+      <c r="D114" s="52"/>
+      <c r="E114" s="52"/>
+      <c r="F114" s="51"/>
+      <c r="G114" s="53"/>
+      <c r="H114" s="53"/>
+      <c r="I114" s="53"/>
+      <c r="J114" s="53"/>
+      <c r="K114" s="53"/>
+      <c r="L114" s="53"/>
+      <c r="M114" s="53"/>
+      <c r="N114" s="53"/>
+      <c r="O114" s="53"/>
     </row>
     <row r="115" spans="2:15" ht="14" customHeight="1">
-      <c r="B115" s="57"/>
-      <c r="C115" s="59"/>
-      <c r="D115" s="59"/>
-      <c r="E115" s="59"/>
-      <c r="F115" s="57"/>
-      <c r="G115" s="60"/>
-      <c r="H115" s="60"/>
-      <c r="I115" s="60"/>
-      <c r="J115" s="60"/>
-      <c r="K115" s="60"/>
-      <c r="L115" s="60"/>
-      <c r="M115" s="60"/>
-      <c r="N115" s="60"/>
-      <c r="O115" s="60"/>
+      <c r="B115" s="51"/>
+      <c r="C115" s="52"/>
+      <c r="D115" s="52"/>
+      <c r="E115" s="52"/>
+      <c r="F115" s="51"/>
+      <c r="G115" s="53"/>
+      <c r="H115" s="53"/>
+      <c r="I115" s="53"/>
+      <c r="J115" s="53"/>
+      <c r="K115" s="53"/>
+      <c r="L115" s="53"/>
+      <c r="M115" s="53"/>
+      <c r="N115" s="53"/>
+      <c r="O115" s="53"/>
     </row>
     <row r="116" spans="2:15" ht="14" customHeight="1">
-      <c r="B116" s="57"/>
-      <c r="C116" s="59"/>
-      <c r="D116" s="59"/>
-      <c r="E116" s="59"/>
-      <c r="F116" s="57"/>
-      <c r="G116" s="60"/>
-      <c r="H116" s="60"/>
-      <c r="I116" s="60"/>
-      <c r="J116" s="60"/>
-      <c r="K116" s="60"/>
-      <c r="L116" s="60"/>
-      <c r="M116" s="60"/>
-      <c r="N116" s="60"/>
-      <c r="O116" s="60"/>
+      <c r="B116" s="51"/>
+      <c r="C116" s="52"/>
+      <c r="D116" s="52"/>
+      <c r="E116" s="52"/>
+      <c r="F116" s="51"/>
+      <c r="G116" s="53"/>
+      <c r="H116" s="53"/>
+      <c r="I116" s="53"/>
+      <c r="J116" s="53"/>
+      <c r="K116" s="53"/>
+      <c r="L116" s="53"/>
+      <c r="M116" s="53"/>
+      <c r="N116" s="53"/>
+      <c r="O116" s="53"/>
     </row>
     <row r="117" spans="2:15" ht="14" customHeight="1">
-      <c r="B117" s="57"/>
-      <c r="C117" s="59"/>
-      <c r="D117" s="59"/>
-      <c r="E117" s="59"/>
-      <c r="F117" s="57"/>
-      <c r="G117" s="60"/>
-      <c r="H117" s="60"/>
-      <c r="I117" s="60"/>
-      <c r="J117" s="60"/>
-      <c r="K117" s="60"/>
-      <c r="L117" s="60"/>
-      <c r="M117" s="60"/>
-      <c r="N117" s="60"/>
-      <c r="O117" s="60"/>
+      <c r="B117" s="51"/>
+      <c r="C117" s="52"/>
+      <c r="D117" s="52"/>
+      <c r="E117" s="52"/>
+      <c r="F117" s="51"/>
+      <c r="G117" s="53"/>
+      <c r="H117" s="53"/>
+      <c r="I117" s="53"/>
+      <c r="J117" s="53"/>
+      <c r="K117" s="53"/>
+      <c r="L117" s="53"/>
+      <c r="M117" s="53"/>
+      <c r="N117" s="53"/>
+      <c r="O117" s="53"/>
     </row>
     <row r="118" spans="2:15" ht="14" customHeight="1">
-      <c r="B118" s="57"/>
-      <c r="C118" s="59"/>
-      <c r="D118" s="59"/>
-      <c r="E118" s="59"/>
-      <c r="F118" s="57"/>
-      <c r="G118" s="60"/>
-      <c r="H118" s="60"/>
-      <c r="I118" s="60"/>
-      <c r="J118" s="60"/>
-      <c r="K118" s="60"/>
-      <c r="L118" s="60"/>
-      <c r="M118" s="60"/>
-      <c r="N118" s="60"/>
-      <c r="O118" s="60"/>
+      <c r="B118" s="51"/>
+      <c r="C118" s="52"/>
+      <c r="D118" s="52"/>
+      <c r="E118" s="52"/>
+      <c r="F118" s="51"/>
+      <c r="G118" s="53"/>
+      <c r="H118" s="53"/>
+      <c r="I118" s="53"/>
+      <c r="J118" s="53"/>
+      <c r="K118" s="53"/>
+      <c r="L118" s="53"/>
+      <c r="M118" s="53"/>
+      <c r="N118" s="53"/>
+      <c r="O118" s="53"/>
     </row>
     <row r="119" spans="2:15" ht="14" customHeight="1">
-      <c r="B119" s="57"/>
-      <c r="C119" s="59"/>
-      <c r="D119" s="59"/>
-      <c r="E119" s="59"/>
-      <c r="F119" s="57"/>
-      <c r="G119" s="60"/>
-      <c r="H119" s="60"/>
-      <c r="I119" s="60"/>
-      <c r="J119" s="60"/>
-      <c r="K119" s="60"/>
-      <c r="L119" s="60"/>
-      <c r="M119" s="60"/>
-      <c r="N119" s="60"/>
-      <c r="O119" s="60"/>
+      <c r="B119" s="51"/>
+      <c r="C119" s="52"/>
+      <c r="D119" s="52"/>
+      <c r="E119" s="52"/>
+      <c r="F119" s="51"/>
+      <c r="G119" s="53"/>
+      <c r="H119" s="53"/>
+      <c r="I119" s="53"/>
+      <c r="J119" s="53"/>
+      <c r="K119" s="53"/>
+      <c r="L119" s="53"/>
+      <c r="M119" s="53"/>
+      <c r="N119" s="53"/>
+      <c r="O119" s="53"/>
     </row>
     <row r="120" spans="2:15" ht="14" customHeight="1">
-      <c r="B120" s="57"/>
-      <c r="C120" s="59"/>
-      <c r="D120" s="59"/>
-      <c r="E120" s="59"/>
-      <c r="F120" s="57"/>
-      <c r="G120" s="60"/>
-      <c r="H120" s="60"/>
-      <c r="I120" s="60"/>
-      <c r="J120" s="60"/>
-      <c r="K120" s="60"/>
-      <c r="L120" s="60"/>
-      <c r="M120" s="60"/>
-      <c r="N120" s="60"/>
-      <c r="O120" s="60"/>
+      <c r="B120" s="51"/>
+      <c r="C120" s="52"/>
+      <c r="D120" s="52"/>
+      <c r="E120" s="52"/>
+      <c r="F120" s="51"/>
+      <c r="G120" s="53"/>
+      <c r="H120" s="53"/>
+      <c r="I120" s="53"/>
+      <c r="J120" s="53"/>
+      <c r="K120" s="53"/>
+      <c r="L120" s="53"/>
+      <c r="M120" s="53"/>
+      <c r="N120" s="53"/>
+      <c r="O120" s="53"/>
     </row>
     <row r="121" spans="2:15" ht="14" customHeight="1">
-      <c r="G121" s="60"/>
-      <c r="H121" s="60"/>
-      <c r="I121" s="60"/>
-      <c r="J121" s="60"/>
-      <c r="K121" s="60"/>
-      <c r="L121" s="60"/>
-      <c r="M121" s="60"/>
-      <c r="N121" s="60"/>
-      <c r="O121" s="60"/>
+      <c r="G121" s="53"/>
+      <c r="H121" s="53"/>
+      <c r="I121" s="53"/>
+      <c r="J121" s="53"/>
+      <c r="K121" s="53"/>
+      <c r="L121" s="53"/>
+      <c r="M121" s="53"/>
+      <c r="N121" s="53"/>
+      <c r="O121" s="53"/>
     </row>
     <row r="122" spans="2:15" ht="14" customHeight="1">
-      <c r="G122" s="60"/>
-      <c r="H122" s="60"/>
-      <c r="I122" s="60"/>
-      <c r="J122" s="60"/>
-      <c r="K122" s="60"/>
-      <c r="L122" s="60"/>
-      <c r="M122" s="60"/>
-      <c r="N122" s="60"/>
-      <c r="O122" s="60"/>
+      <c r="G122" s="53"/>
+      <c r="H122" s="53"/>
+      <c r="I122" s="53"/>
+      <c r="J122" s="53"/>
+      <c r="K122" s="53"/>
+      <c r="L122" s="53"/>
+      <c r="M122" s="53"/>
+      <c r="N122" s="53"/>
+      <c r="O122" s="53"/>
     </row>
     <row r="123" spans="2:15" ht="14" customHeight="1">
-      <c r="G123" s="60"/>
-      <c r="H123" s="60"/>
-      <c r="I123" s="60"/>
-      <c r="J123" s="60"/>
-      <c r="K123" s="60"/>
-      <c r="L123" s="60"/>
-      <c r="M123" s="60"/>
-      <c r="N123" s="60"/>
-      <c r="O123" s="60"/>
+      <c r="G123" s="53"/>
+      <c r="H123" s="53"/>
+      <c r="I123" s="53"/>
+      <c r="J123" s="53"/>
+      <c r="K123" s="53"/>
+      <c r="L123" s="53"/>
+      <c r="M123" s="53"/>
+      <c r="N123" s="53"/>
+      <c r="O123" s="53"/>
     </row>
     <row r="124" spans="2:15" ht="14" customHeight="1">
-      <c r="G124" s="60"/>
-      <c r="H124" s="60"/>
-      <c r="I124" s="60"/>
-      <c r="J124" s="60"/>
-      <c r="K124" s="60"/>
-      <c r="L124" s="60"/>
-      <c r="M124" s="60"/>
-      <c r="N124" s="60"/>
-      <c r="O124" s="60"/>
+      <c r="G124" s="53"/>
+      <c r="H124" s="53"/>
+      <c r="I124" s="53"/>
+      <c r="J124" s="53"/>
+      <c r="K124" s="53"/>
+      <c r="L124" s="53"/>
+      <c r="M124" s="53"/>
+      <c r="N124" s="53"/>
+      <c r="O124" s="53"/>
     </row>
     <row r="125" spans="2:15" ht="14" customHeight="1">
-      <c r="G125" s="60"/>
-      <c r="H125" s="60"/>
-      <c r="I125" s="60"/>
-      <c r="J125" s="60"/>
-      <c r="K125" s="60"/>
-      <c r="L125" s="60"/>
-      <c r="M125" s="60"/>
-      <c r="N125" s="60"/>
-      <c r="O125" s="60"/>
+      <c r="G125" s="53"/>
+      <c r="H125" s="53"/>
+      <c r="I125" s="53"/>
+      <c r="J125" s="53"/>
+      <c r="K125" s="53"/>
+      <c r="L125" s="53"/>
+      <c r="M125" s="53"/>
+      <c r="N125" s="53"/>
+      <c r="O125" s="53"/>
     </row>
     <row r="126" spans="2:15" ht="14" customHeight="1">
-      <c r="G126" s="60"/>
-      <c r="H126" s="60"/>
-      <c r="I126" s="60"/>
-      <c r="J126" s="60"/>
-      <c r="K126" s="60"/>
-      <c r="L126" s="60"/>
-      <c r="M126" s="60"/>
-      <c r="N126" s="60"/>
-      <c r="O126" s="60"/>
+      <c r="G126" s="53"/>
+      <c r="H126" s="53"/>
+      <c r="I126" s="53"/>
+      <c r="J126" s="53"/>
+      <c r="K126" s="53"/>
+      <c r="L126" s="53"/>
+      <c r="M126" s="53"/>
+      <c r="N126" s="53"/>
+      <c r="O126" s="53"/>
     </row>
     <row r="127" spans="2:15" ht="14" customHeight="1">
-      <c r="G127" s="60"/>
-      <c r="H127" s="60"/>
-      <c r="I127" s="60"/>
-      <c r="J127" s="60"/>
-      <c r="K127" s="60"/>
-      <c r="L127" s="60"/>
-      <c r="M127" s="60"/>
-      <c r="N127" s="60"/>
-      <c r="O127" s="60"/>
+      <c r="G127" s="53"/>
+      <c r="H127" s="53"/>
+      <c r="I127" s="53"/>
+      <c r="J127" s="53"/>
+      <c r="K127" s="53"/>
+      <c r="L127" s="53"/>
+      <c r="M127" s="53"/>
+      <c r="N127" s="53"/>
+      <c r="O127" s="53"/>
     </row>
     <row r="128" spans="2:15" ht="14" customHeight="1">
-      <c r="G128" s="60"/>
-      <c r="H128" s="60"/>
-      <c r="I128" s="60"/>
-      <c r="J128" s="60"/>
-      <c r="K128" s="60"/>
-      <c r="L128" s="60"/>
-      <c r="M128" s="60"/>
-      <c r="N128" s="60"/>
-      <c r="O128" s="60"/>
+      <c r="G128" s="53"/>
+      <c r="H128" s="53"/>
+      <c r="I128" s="53"/>
+      <c r="J128" s="53"/>
+      <c r="K128" s="53"/>
+      <c r="L128" s="53"/>
+      <c r="M128" s="53"/>
+      <c r="N128" s="53"/>
+      <c r="O128" s="53"/>
     </row>
     <row r="129" spans="7:15" ht="14" customHeight="1">
-      <c r="G129" s="60"/>
-      <c r="H129" s="60"/>
-      <c r="I129" s="60"/>
-      <c r="J129" s="60"/>
-      <c r="K129" s="60"/>
-      <c r="L129" s="60"/>
-      <c r="M129" s="60"/>
-      <c r="N129" s="60"/>
-      <c r="O129" s="60"/>
+      <c r="G129" s="53"/>
+      <c r="H129" s="53"/>
+      <c r="I129" s="53"/>
+      <c r="J129" s="53"/>
+      <c r="K129" s="53"/>
+      <c r="L129" s="53"/>
+      <c r="M129" s="53"/>
+      <c r="N129" s="53"/>
+      <c r="O129" s="53"/>
     </row>
     <row r="130" spans="7:15" ht="14" customHeight="1">
-      <c r="G130" s="60"/>
-      <c r="H130" s="60"/>
-      <c r="I130" s="60"/>
-      <c r="J130" s="60"/>
-      <c r="K130" s="60"/>
-      <c r="L130" s="60"/>
-      <c r="M130" s="60"/>
-      <c r="N130" s="60"/>
-      <c r="O130" s="60"/>
+      <c r="G130" s="53"/>
+      <c r="H130" s="53"/>
+      <c r="I130" s="53"/>
+      <c r="J130" s="53"/>
+      <c r="K130" s="53"/>
+      <c r="L130" s="53"/>
+      <c r="M130" s="53"/>
+      <c r="N130" s="53"/>
+      <c r="O130" s="53"/>
     </row>
     <row r="131" spans="7:15" ht="14" customHeight="1">
-      <c r="G131" s="60"/>
-      <c r="H131" s="60"/>
-      <c r="I131" s="60"/>
-      <c r="J131" s="60"/>
-      <c r="K131" s="60"/>
-      <c r="L131" s="60"/>
-      <c r="M131" s="60"/>
-      <c r="N131" s="60"/>
-      <c r="O131" s="60"/>
+      <c r="G131" s="53"/>
+      <c r="H131" s="53"/>
+      <c r="I131" s="53"/>
+      <c r="J131" s="53"/>
+      <c r="K131" s="53"/>
+      <c r="L131" s="53"/>
+      <c r="M131" s="53"/>
+      <c r="N131" s="53"/>
+      <c r="O131" s="53"/>
     </row>
     <row r="132" spans="7:15" ht="14" customHeight="1">
-      <c r="G132" s="60"/>
-      <c r="H132" s="60"/>
-      <c r="I132" s="60"/>
-      <c r="J132" s="60"/>
-      <c r="K132" s="60"/>
-      <c r="L132" s="60"/>
-      <c r="M132" s="60"/>
-      <c r="N132" s="60"/>
-      <c r="O132" s="60"/>
+      <c r="G132" s="53"/>
+      <c r="H132" s="53"/>
+      <c r="I132" s="53"/>
+      <c r="J132" s="53"/>
+      <c r="K132" s="53"/>
+      <c r="L132" s="53"/>
+      <c r="M132" s="53"/>
+      <c r="N132" s="53"/>
+      <c r="O132" s="53"/>
     </row>
     <row r="133" spans="7:15" ht="14" customHeight="1">
-      <c r="G133" s="60"/>
-      <c r="H133" s="60"/>
-      <c r="I133" s="60"/>
-      <c r="J133" s="60"/>
-      <c r="K133" s="60"/>
-      <c r="L133" s="60"/>
-      <c r="M133" s="60"/>
-      <c r="N133" s="60"/>
-      <c r="O133" s="60"/>
+      <c r="G133" s="53"/>
+      <c r="H133" s="53"/>
+      <c r="I133" s="53"/>
+      <c r="J133" s="53"/>
+      <c r="K133" s="53"/>
+      <c r="L133" s="53"/>
+      <c r="M133" s="53"/>
+      <c r="N133" s="53"/>
+      <c r="O133" s="53"/>
     </row>
     <row r="134" spans="7:15" ht="14" customHeight="1">
-      <c r="G134" s="60"/>
-      <c r="H134" s="60"/>
-      <c r="I134" s="60"/>
-      <c r="J134" s="60"/>
-      <c r="K134" s="60"/>
-      <c r="L134" s="60"/>
-      <c r="M134" s="60"/>
-      <c r="N134" s="60"/>
-      <c r="O134" s="60"/>
+      <c r="G134" s="53"/>
+      <c r="H134" s="53"/>
+      <c r="I134" s="53"/>
+      <c r="J134" s="53"/>
+      <c r="K134" s="53"/>
+      <c r="L134" s="53"/>
+      <c r="M134" s="53"/>
+      <c r="N134" s="53"/>
+      <c r="O134" s="53"/>
     </row>
     <row r="135" spans="7:15" ht="14" customHeight="1">
-      <c r="G135" s="60"/>
-      <c r="H135" s="60"/>
-      <c r="I135" s="60"/>
-      <c r="J135" s="60"/>
-      <c r="K135" s="60"/>
-      <c r="L135" s="60"/>
-      <c r="M135" s="60"/>
-      <c r="N135" s="60"/>
-      <c r="O135" s="60"/>
+      <c r="G135" s="53"/>
+      <c r="H135" s="53"/>
+      <c r="I135" s="53"/>
+      <c r="J135" s="53"/>
+      <c r="K135" s="53"/>
+      <c r="L135" s="53"/>
+      <c r="M135" s="53"/>
+      <c r="N135" s="53"/>
+      <c r="O135" s="53"/>
     </row>
     <row r="136" spans="7:15" ht="14" customHeight="1">
-      <c r="G136" s="60"/>
-      <c r="H136" s="60"/>
-      <c r="I136" s="60"/>
-      <c r="J136" s="60"/>
-      <c r="K136" s="60"/>
-      <c r="L136" s="60"/>
-      <c r="M136" s="60"/>
-      <c r="N136" s="60"/>
-      <c r="O136" s="60"/>
+      <c r="G136" s="53"/>
+      <c r="H136" s="53"/>
+      <c r="I136" s="53"/>
+      <c r="J136" s="53"/>
+      <c r="K136" s="53"/>
+      <c r="L136" s="53"/>
+      <c r="M136" s="53"/>
+      <c r="N136" s="53"/>
+      <c r="O136" s="53"/>
     </row>
     <row r="137" spans="7:15" ht="14" customHeight="1">
-      <c r="G137" s="60"/>
-      <c r="H137" s="60"/>
-      <c r="I137" s="60"/>
-      <c r="J137" s="60"/>
-      <c r="K137" s="60"/>
-      <c r="L137" s="60"/>
-      <c r="M137" s="60"/>
-      <c r="N137" s="60"/>
-      <c r="O137" s="60"/>
+      <c r="G137" s="53"/>
+      <c r="H137" s="53"/>
+      <c r="I137" s="53"/>
+      <c r="J137" s="53"/>
+      <c r="K137" s="53"/>
+      <c r="L137" s="53"/>
+      <c r="M137" s="53"/>
+      <c r="N137" s="53"/>
+      <c r="O137" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4008,7 +4128,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4024,7 +4144,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4032,7 +4152,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -4060,15 +4180,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="67"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="19" t="s">

</xml_diff>